<commit_message>
Upload stage 3 evidence for B1-B2
</commit_message>
<xml_diff>
--- a/techwomen35/evidence.xlsx
+++ b/techwomen35/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\1W_techwomen35\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0k_techwomen35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52EA609-92FB-4CA0-BB63-0B00320F9194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157E8CEC-75EB-4377-8B4A-7CB0E93C2571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="894" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
   <si>
     <t>TxHash</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>589A52140367B1894E1F3FC88CE632CB87FAB92E393DE4D1A02E522B0ACF93AD</t>
+  </si>
+  <si>
+    <t>E5AD0CE00693DB7C9226CB84BC5E3CC5755CE283C76712AD412EA4F5C91542E8</t>
+  </si>
+  <si>
+    <t>03F24C1272F863EA37124400DE343E3C64263B822A38ED597443C7FAB86BA048</t>
+  </si>
+  <si>
+    <t>400486D619EE56A7068F348F8EF0BF80EEA9C665BBBAFF2BDBB68217E71EFE51</t>
+  </si>
+  <si>
+    <t>486586F1DEB8FE28694CB4FE0AEF4A80CA17F4BE537359E82440EFB277B6E741</t>
   </si>
 </sst>
 </file>
@@ -581,8 +593,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1236,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1238,12 +1252,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1272,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1272,12 +1288,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload stage 2 evidence for A7-A20
</commit_message>
<xml_diff>
--- a/techwomen35/evidence.xlsx
+++ b/techwomen35/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0k_techwomen35\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0k_techwomen35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157E8CEC-75EB-4377-8B4A-7CB0E93C2571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5026CD6-62EA-49FC-8EDE-203016074FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="894" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="2160" windowWidth="21600" windowHeight="11385" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="94">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,27 +58,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -188,13 +173,166 @@
   </si>
   <si>
     <t>486586F1DEB8FE28694CB4FE0AEF4A80CA17F4BE537359E82440EFB277B6E741</t>
+  </si>
+  <si>
+    <t>ibc/C8BA5D98E29C7E663ED1C9BB4992B5FC8B5C4F35498E642E836E5E6B4230D816</t>
+  </si>
+  <si>
+    <t>techwomensA7</t>
+  </si>
+  <si>
+    <t>ibc/85CF5AD72D9EF5BAE228749578AE6688B20BBCD4C54441C1707CAC408D530A6F</t>
+  </si>
+  <si>
+    <t>techwomensA8</t>
+  </si>
+  <si>
+    <t>ibc/83BF87DC75D17C50B3B32DD731625B6831C13CF9852D58EE63DC33EA40E10F8C</t>
+  </si>
+  <si>
+    <t>techwomensA9</t>
+  </si>
+  <si>
+    <t>ibc/3DAB18CF7292778B2D25D55890D971B98FFB8376F5855471086D72B8DC3FE5A6</t>
+  </si>
+  <si>
+    <t>techwomensA10</t>
+  </si>
+  <si>
+    <t>ibc/18E3ADEB34DF7FFD5E3B9D93E1A5942F7E4D6D3108A4400AF852CFFC29FAF4EE</t>
+  </si>
+  <si>
+    <t>techwomensA11</t>
+  </si>
+  <si>
+    <t>ibc/01CDDC043A83AFE81B2449A9C2327DF902C9875B9270A766321C77533886AAEB</t>
+  </si>
+  <si>
+    <t>techwomensA12</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>DF9F45E6654649A9CCAA71DB2562D79CAA5A9BC813DEB692DA3D8965AC849927</t>
+  </si>
+  <si>
+    <t>3FB24E951CAB2F24AFE912C2D40C3597234DBF008BC86200D91198F816DED1E5</t>
+  </si>
+  <si>
+    <t>2BECFF762B709967D857BCCF7DF4F1D0A56978AD7AA09CEC980FC2906BFACCEB</t>
+  </si>
+  <si>
+    <t>B1F1B03C77996218CDE83D960685AEB101EBFEBB033A6A74542D16CBAE955F3E</t>
+  </si>
+  <si>
+    <t>FD0DFB314C73E29BE819DA9959166753380BADDC5E15D559311F5E37C28E00B7</t>
+  </si>
+  <si>
+    <t>476809197DC57212C890FFA74482DBFC7A24D31C36073E356BD130437DFD9D58</t>
+  </si>
+  <si>
+    <t>83416B682DD37410C9E85AB0790AE0C8468D099708B165829DB2D805B130B292</t>
+  </si>
+  <si>
+    <t>EAE38E4AF1E4279551A60929610C86108DCB2D30D708170DA0D5A3ED1513B5B6</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>2CF9CED1D7B8E52DF5B5CCCCDBC3AACCD06E960C61EE857F9D7624D30309B837</t>
+  </si>
+  <si>
+    <t>9B9F74B4A31C5211EE7C65ED1FA676F675A08497D5C605C179EBEA87D526B2D3</t>
+  </si>
+  <si>
+    <t>36544FA0BE4B4471CCC90CF32B50E767CC26675E5236428C9258FCF6D3C1895D</t>
+  </si>
+  <si>
+    <t>D3CCB44F5702518DF4EBC1789FC16CB389378F9BBA194A5F2DB8B1FF64C3F9AF</t>
+  </si>
+  <si>
+    <t>FE0299B1B6D0AFAD97886169189BC22B53F2A3F637FEA25BF613769A035C659F</t>
+  </si>
+  <si>
+    <t>F2C58557FC2FAFBAF1A9E763C060C96D1F1F79758C2EBB5D00EEB788FB47439E</t>
+  </si>
+  <si>
+    <t>21ED153C616C8CCDCDA7CA3D39587C4AEC93BD6F1D1D8222EC8FD993D12346CC</t>
+  </si>
+  <si>
+    <t>1A7F215A622DA15CA021BE70F9DA59E954330F3BDD51490B49588939B87B63BF</t>
+  </si>
+  <si>
+    <t>C9AF1865F3CE6E57DF400C5511BD0C9CF86121071FEE97D93C21CCF82ED30E85</t>
+  </si>
+  <si>
+    <t>E96727C99AF7D2F1D8E3CBFDC192E4049643A8AD556C7E951F193E6F3680C8B7</t>
+  </si>
+  <si>
+    <t>6198B2FBA6DCBAF1473D93C87ADE1F6B38FC309C45BB17222563C7F73A317CC6</t>
+  </si>
+  <si>
+    <t>63BC07A6EF517AD9DCCED306122F7E10D30F7D9D89BB6F3EE63E883E60EE9A7F</t>
+  </si>
+  <si>
+    <t>89D82A8E59A4CE91A102CF51D0BAED19605C4C8865035317081D801CDDB02CAB</t>
+  </si>
+  <si>
+    <t>565EBEB6FAC0E6C0DD35BAA99AFD4FF40D01DDA0BD1ABF19E8B24BB0D8A37CB8</t>
+  </si>
+  <si>
+    <t>040C451DABD208FD44585727023541ACD8978D53AF2C7F1FE6BF40F902C4FA73</t>
+  </si>
+  <si>
+    <t>8AD7B144A8A1A9041E52C51E1BDEBAA6A6547C0FB2E4373E479C31A7292E079F</t>
+  </si>
+  <si>
+    <t>63E61ADEBABB85ECE83F9CAA4D25B11525FA3A98B85B14B3D83AAF8D182635FF</t>
+  </si>
+  <si>
+    <t>1065607D0979449DAF53D2BE8361E88839DF2F5629306AAACA573071DE9A91F4</t>
+  </si>
+  <si>
+    <t>1B854C0147E83EA814BF6AA5CE624AE227696309F1A6B9E7FCE46CEEC27728EA</t>
+  </si>
+  <si>
+    <t>679E5E18AEFA651495F0A6E0F7F78F88F87AD37ACC879C4E527F1F85A551D7DC</t>
+  </si>
+  <si>
+    <t>EF3706641967197D0C9B79AFDEFAE96E129246EE815B074A17EB59B443949543</t>
+  </si>
+  <si>
+    <t>04D14051EB029676E5806CD96180936ACF9C2F2B7713F93F54779FC472A853E4</t>
+  </si>
+  <si>
+    <t>012F08C95BA663A79D7C67D396972C1D66FC89E7951A05120328E69C22D66E46</t>
+  </si>
+  <si>
+    <t>BA1A5C65D4E7BF2891402C37ED4C6A5B887EAFA5144F7D8CBDF964ADB8369778</t>
+  </si>
+  <si>
+    <t>AC13A83521480B1DB2CC35C73BAA177784A8C5615C0CF1D6659A63DBAC3BC23A</t>
+  </si>
+  <si>
+    <t>91FF08AAC9389F6B5319B15A44C42B20C730EB2257AD7453BCB927505D164FC9</t>
+  </si>
+  <si>
+    <t>D2DEED0C5E0ECE3CD1B001673B45D20F92BA262AF6333EA6C8B9199C61F69D99</t>
+  </si>
+  <si>
+    <t>729040CF0AF08B6090D0236950F8B70FF7B33DFAFC37BC9369A6EE7280435B1E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +351,34 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="4">
@@ -264,10 +430,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -286,9 +455,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{363F736F-3FC9-478F-926C-793540997E34}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{C73D49A6-9D0A-4863-9645-9089DC2260EB}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{4529E2D8-5151-4684-81C3-2355A4AA06C8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -593,8 +772,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,51 +790,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -671,7 +850,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -681,33 +862,558 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -717,33 +1423,75 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -753,78 +1501,6 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -832,397 +1508,52 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1252,12 +1583,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1272,7 +1603,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -1288,12 +1619,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1391,54 +1722,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1470,10 +1801,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1481,16 +1812,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1521,10 +1852,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1532,16 +1863,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1572,10 +1903,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1583,16 +1914,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1624,10 +1955,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1635,16 +1966,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1659,7 +1990,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1669,18 +2002,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1695,7 +2028,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1705,18 +2040,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>